<commit_message>
Improve mock data generation
</commit_message>
<xml_diff>
--- a/BE-mh-narrative-dashboard/generate_mock_data/context/INS-W_963_full_all_encounters.xlsx
+++ b/BE-mh-narrative-dashboard/generate_mock_data/context/INS-W_963_full_all_encounters.xlsx
@@ -10,7 +10,6 @@
     <sheet name="enc_1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="enc_2" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="enc_3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="enc_4" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -428,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,140 +450,384 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Hello Mei Lin, I appreciate you coming in today. I’d like to start by understanding a bit more about how you’ve been feeling lately. Could you tell me what’s been going on for you recently, especially with your mood or energy levels?</t>
+          <t>Hi Gabriella, I understand that you're here today because you've been experiencing some low mood.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Um, hi... Yeah, I guess I've been feeling really tired all the time. Like, I don’t have the energy to do anything, even things I used to enjoy. It’s hard to concentrate in class, and I just feel kind of... heavy, I guess. Sometimes, I don’t even want to get out of bed. It’s been like this for a while now, and it’s making everything harder.</t>
+          <t>Yeah, I just recently I've just... I'm just feeling down a lot and I can't really, like, snap out of it. Like, sometimes if it's happened before, I can just, like, get myself back on track. But recently I'm just finding it really difficult to do.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>It sounds like you're experiencing persistent fatigue, difficulty concentrating, and a sense of heaviness that’s been affecting your daily life for some time. When you mention feeling like you don’t want to get out of bed, do you also notice any changes in your sleep patterns—like sleeping more than usual, or having trouble sleeping?</t>
+          <t>So it sounds like you've been experiencing some low mood and you're kind of struggling to get going a bit.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Yeah... I think I’ve been sleeping a lot, but still feeling tired when I wake up. Sometimes, I just can’t fall asleep at all, and I stay up all night. Other times, I sleep for hours, but it doesn’t really feel restful. It’s like my sleep isn’t helping me feel better. I don’t know if it’s related, but I’ve been having more headaches too.</t>
+          <t>Yeah, definitely.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>It sounds like your sleep has been quite disrupted, and even when you do sleep, it doesn’t seem to restore your energy. You also mentioned experiencing more headaches. Given these symptoms—persistent fatigue, sleep difficulties, headaches, and heaviness—how long have you been noticing these changes? Did anything recently happen that might have triggered or worsened these feelings?</t>
+          <t>You've had low mood in the past, but it's kind of... you've been able to pull yourself out of it before, but more recently you've found that harder. Okay, so I understand that you first went to your GP, who referred you here about two months ago. Can I ask what led you to go to the GP in the first place?</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Hmm, I think it’s been going on for a few months now. Maybe since the start of the semester. As for what triggered it, I guess the stress from school has been worse lately. I’ve been feeling more overwhelmed with exams and deadlines. Plus, I’ve been feeling more alone, even though I’m around people most of the time.</t>
+          <t>My long-term boyfriend broke up with me and it was, it was such a shock, like I really wasn't expecting it. It just got me really down. I felt really lonely. And I didn't really want to see people. I just wanted to be in my own space. My mom told me I should probably go to the doctors and he's referred me to you.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Thank you for sharing that, Mei Lin. It sounds like the academic pressures and feelings of loneliness have increased recently, which might be contributing to how you're feeling physically and emotionally. When you mention feeling overwhelmed and alone, can you tell me more about your social interactions and your support system? Do you have friends or family you feel comfortable talking to about these feelings?</t>
+          <t>Okay? So it sounds like you had that breakup and you weren't expecting it, so it kind of came out of the blue a bit and you've been on your own quite a lot. So you're not been seeing people as much. And it sounds like your mum noticed that there's been a bit of a change in you. Okay, and how have things been then since then, since that happened and since you went to the GP?</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Honestly, I don’t really talk about this kind of stuff with anyone. I have a few friends, but I don’t want to burden them, so I just keep it to myself. My family is far away, and I don’t think they really understand what I’m going through. Sometimes I feel like I’m just pretending to be okay around others. It’s like, I’m alone even when I’m around people.</t>
+          <t>I just, nothing's really changed. Nothing's really improved. I just... I feel down, like everything's an effort and feel distant from things. And like I said, I can't snap out of it.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>It sounds like you’re carrying a lot on your own, feeling hesitant to share your struggles because you don’t want to burden others, and perhaps feeling misunderstood by your family. That sense of loneliness can be really tough to handle, especially when you're trying to manage everything on your own. 
-Given what you've shared so far—persistent fatigue, sleep problems, headaches, feelings of heaviness, and loneliness—how do you feel these issues are affecting your daily life, like your studies or your ability to engage in activities you used to enjoy?</t>
+          <t>Okay, and how did you feel about coming here today?</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>It's like, I’m so overwhelmed, but I don’t really have the energy or motivation to do anything. Classes feel harder, and I can’t focus on my homework. Even when I want to go out with friends or do something fun, I just can’t bring myself to do it. It’s like I’m stuck in this cycle where everything feels heavy and pointless. Sometimes I wonder if I’m just not cut out for all of this.</t>
+          <t>I was kind of disappointed in myself because I feel like nobody else my age is doing this. I should have been able to snap out of it, like it's just another thing that I've not really... you know, things that's making me stand out for the wrong reasons.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>That sounds incredibly challenging, Mei Lin. Feeling overwhelmed and lacking motivation can really make daily life feel like a struggle, and your sense of everything being heavy and pointless is a serious concern. It's understandable to question your abilities when you're going through such a tough time. 
-Given these feelings and the physical symptoms you've described, have you noticed if your mood has changed in other ways—like feelings of sadness, hopelessness, or lack of interest in things you used to enjoy? Or perhaps thoughts that worry you about the future?</t>
+          <t>Okay, so you feel like it's kind of odd or unusual to be coming to see a clinical psychologist. I suppose I just want to reassure you that it's absolutely normal to have feelings of depression and anxiety. It's really very common, and it certainly isn't odd or strange at all. So it sounds like it was actually quite hard for you to come here today. So what I guess led you to do that? Because it sounds like maybe there was a lot pushing you against coming here today, but you've managed to come anyway.</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Yeah, I guess I do feel more sad lately. Sometimes, I just feel like nothing’s going to get better, and I don’t see a way out. I used to enjoy studying biology, but now I can’t even focus on that. I’ve had some thoughts about giving up, but I don’t know if that’s normal or not. It’s like, I don’t really see the point anymore.</t>
+          <t>I'm just hoping that it's going to help. I think I didn't really want to admit it because, like, it's just another failure, but my mum was talking to me and she's not really happy with the way I'm behaving. I didn't really want to disappoint her again. And so I thought there's no harm in it. So I came.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Thank you for being honest about these feelings, Mei Lin. It’s really important to acknowledge these thoughts, especially when they involve feelings of hopelessness or thoughts about giving up. They can be signs that you're going through a depressive episode, which is quite common in situations like yours, especially with the stress and isolation you're experiencing.
-Would you be comfortable talking more about these thoughts? For example, what do you mean by “giving up,” and how often do these thoughts come up? Understanding this can help us figure out the best way to support you.</t>
+          <t>So it sounds like partly you're doing it then for your mum because you're a bit worried that she isn't pleased with you at the moment.</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Um, I don’t know... I guess I think about just not trying anymore. Like, just stopping everything—school, everything I do. Sometimes, I feel like it wouldn’t matter if I was here or not. These thoughts come more often when I’m feeling really low, especially late at night. I don’t want to scare myself, but it’s hard to ignore them.</t>
+          <t>Yeah.</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Thank you for sharing that, Mei Lin. It’s very brave of you to talk about these thoughts. When you mention feeling like it wouldn’t matter if you were here, and that these thoughts come more often when you're feeling low, it suggests that you're experiencing some very difficult feelings right now. 
-It's important to remember that these thoughts are symptoms of depression, and they can be very distressing. You’re not alone in this, and there are ways to help you through these feelings. 
-Given everything you've described — the fatigue, sleep issues, headaches, feelings of sadness, and thoughts about giving up — it seems like you’re experiencing a significant level of distress. Would you be open to exploring some strategies to cope with these feelings and perhaps discuss some options for support?</t>
+          <t>Well, I think it's great that you've come here. And definitely there's a lot of evidence to suggest that psychological therapy can help depression, and particularly the type of therapy that we're gonna be doing, which is called cognitive behavior therapy. I'll tell you a bit more about that as we go on, but I'm just trying to find out a bit more about you today. So I saw from your notes that you're a medic student.</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>I guess I’m willing to listen... I don’t really know what else to do. Nothing’s really helped so far, and I feel like I’m just stuck in this place.</t>
+          <t>Yeah? I'm not currently in uni at the moment, but yeah, last year I was a medical student.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>It’s understandable to feel that way, Mei Lin. Feeling stuck can be really discouraging, especially when it seems like nothing has helped so far. But reaching out today is a positive step, and together we can explore ways to help you feel better and find some relief from these overwhelming feelings. 
-In our next steps, I’d like to understand more about what has and hasn’t worked for you in the past, and discuss some strategies that might help improve your mood and energy levels. Does that sound okay to you?</t>
+          <t>Okay, so I guess why, what's the reason that you're not in uni this year?</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Yeah, that sounds okay. I just want to feel a little better, even if it’s just a little.</t>
+          <t>It was pretty tough first year, so they then suggested that I took a year out. This is the break.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>That’s a very good goal, Mei Lin. Even small improvements can make a meaningful difference in how you’re feeling. Before we move forward, I’d like to briefly review some of the information you’ve shared today—your feelings of fatigue, sleep disturbances, headaches, sadness, and thoughts of giving up. 
-Based on what you’ve told me, it seems like you’re experiencing symptoms that are consistent with depression, which is common among people facing significant stress and isolation. Our goal will be to work together to find strategies that can help you manage these symptoms and improve your overall well-being.
-In our next session, we can explore specific coping skills, possibly including behavioral strategies, and discuss whether additional support or treatment options might be helpful. Does that sound like a good plan for now?</t>
+          <t>Okay, so just thinking, so that would be about 6 months ago, was it that your year out started? And it sounds then maybe like your first year was also quite tough?</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Yes, that sounds good. Thank you for listening and understanding. I appreciate it.</t>
+          <t>Yeah, it was. I thought it's tough for everyone, but obviously we all take it in different ways, don't we.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>You're very welcome, Mei Lin. I'm glad you felt comfortable sharing today. Remember, you're not alone in this, and help is available. We'll work together to find ways to support you through these feelings. I look forward to our next session. See you next time.</t>
+          <t>And you're planning on returning?</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Goodbye.</t>
+          <t>Yeah, I'm going to have to really.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>But you don't sound too sure about that.</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>No, though I think returning is probably... that's what's going to make everyone happy. And I think, you know, at least I'll be able to finally achieve something and get something right. So yeah, like next year I'm going to... I'll get through that. Yeah.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Okay, so it doesn't sound like you want to go back.</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>I do. I didn't enjoy it. I just... I just don't feel like me at the moment. And I just, it's a lot of work. It's a lot of pressure. But that's what comes with it. And, you know, it'll work out for the best if I go.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Okay, so I guess then there's quite a lot of thoughts and feelings about going back at the moment. I'm just wondering, in the meantime, what are you up to, what have you been doing?</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Well, I haven't really had much on the horizon. My mom, her friends own a restaurant and she suggested that I did a bit of waitressing there, just doing it for a bit of money and stuff because obviously I'm not in uni, so you know, I've done that.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Okay, how many shifts have you done there?</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>I've only done one so far. Yeah, I don't know whether it's something that I'd probably go back to.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Okay, when was that shift?</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>It was last week, actually.</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Okay, and how was it? I suppose I'm intrigued, can you tell me a bit more about that?</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>It was, it was different, you know, because it was like... I did enjoy it because it's just a different aspect and I had to speak to people and try to get their orders and try to remember it and stuff. I wasn't very good, but I suppose it was handy to have some money, like get out of the house.</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>So it sounds like you quite enjoyed that. Then what makes you think you weren't very good?</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>I just felt slow. And people, sometimes they didn't understand what I was saying, so I'd have to talk louder or quieter, slower. And I got a bit confused sometimes with the orders, and I just don't really think that I'm not really like a friendly... like people don't really think that I'm a friendly person, so they didn't really want to talk to me and stuff. I felt like I was inconveniencing them, by like asking them things and getting things wrong. Yeah, they said that apparently most people get like a few mistakes on their first shift, but then again, she's my mom's friend, so that's probably why she's saying it.</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>So the person who owns the restaurant is your mum's friend. Okay, so you're saying that you think you weren't very good, and that's because you were a bit slow and you got confused with some orders. But you said it's common for people to do that on that first shift. That's what she said to you, but...</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>But it's probably just she's just trying to make me feel better. She probably felt sorry for me because I'm obviously not very good at it, like I'm not very good at anything recently. I think she just felt sorry for me.</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Okay, so I've just been noting down some of those thoughts that you've been having. You kind of say that you feel like you're not very good, you're slow, you're confused with the orders, and you feel like you're inconveniencing her and she feels sorry for you. I suppose I'm wondering, I mean, what makes you think that she feels sorry for you?</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Like I said, she's my mum's friend, and she's obviously feeling sorry for my mum as well because she's got a daughter that's not like anyone else of her age. And she's just like all alone and she's not getting involved. So I think she just feels sorry for me and she doesn't want, like, to upset me. But yeah.</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>When you're having these kind of thoughts, because that's quite a lot of negative thoughts you're describing, how do you feel?</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Just feel empty, I don't... I'm just calling as it is. I'm just calling it as reality. I feel like I'm being honest with myself by just voicing it and not trying to get around hiding it because I know, like, I can see it in myself.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>So it sounds like you feel like those thoughts are very true then? I mean, if you were going to write them... So I'm going to pick out some of those thoughts you describe. You said 'I'm not very good', and 'I'm inconveniencing them'. How much would you say you believe those on a scale out of 100, where 100 is like, I absolutely believe it and 0 is like, I don't believe it at all?</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>I'm about 80, yeah.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>So you feel quite sure that you definitely believe those, okay? And you said that when you're thinking those thoughts, you start to feel quite empty.</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>I just feel distant and like I said, I'm not really myself, I just... It's like I'm not really there, but when I am, I can't even do a good job.</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>And are there any other emotions that you experience?</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>I feel drained. I'd say I feel like I'm not in touch with anything, just... it's like everything's going on around me, but I'm just not there. I'm just, it's like I'm just watching.</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Okay, so you feel empty, distant, you feel drained. And how, when you're feeling these emotions, how do you feel in your body? Kind of what sensations do you notice?</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>I don't know how to describe it. I get like, I have a bit of like, like, you know, when you kind of get like butterflies when you're nervous and stuff, kind of get a bit of that.</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>You feel some butterflies? Yeah, did you have butterflies that night when you were at the restaurant?</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Yeah, I was pretty nervous. Then when I got into it, they went away and like it distracted me for a bit. And so obviously I realized that I wasn't doing a very good job.</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Okay? And you, when you have those emotions, how does it affect your energy levels? Do you feel more energetic, less energetic, or about the same when you feel down?</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Yeah, when you're having those emotions that you were describing... I just feel drained, like didn't even have like the energy to wake up in the morning sometimes, like I just felt pointless, like my body's heavy and I don't want to. Yeah.</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>So it sounds like you feel very tired. You're struggling to wake up. You said it's pointless. And what do you do then when you feel like that? So I guess you just talked about when you wake up in the morning and you feel heavy, and I suppose you've been maybe having some of these thoughts and those emotions potentially the night before, what do you then do? How do you respond to that?</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>I just have to get up I suppose. I don't really have a choice because my mum, I live with my mom. I know it's hard for her, so I don't want her to be too worried. So I just... I just try to carry on as normal. It takes longer and I don't want to, but I do, so I'll go on with my routine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>So you're a bit slower in getting up, but you are still getting up anyway. And what about your kind of, what do you think about when you're doing that?</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>I'm just thinking that nobody else is like me my age, like nobody should be feeling like this. And I'm the only one that does.</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>So it sounds like you think a bit more about the problem and you kind of spend time thinking about...</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>How I hate it and I don't want to feel like this, but I do, and nobody else I know does. So it makes me feel even more alone and like getting me even more down. And I just don't want to disappoint anyone. I didn't really want it.</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Okay, so it sounds like you're trying to toughen up on yourself a little bit, tell yourself to work harder, to be different.</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Okay.</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>And when you start telling yourself that kind of thing, how does that make you feel? Does that make you feel better afterwards or worse?</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Feels worse. Because I still can't snap out of it, like I'm aware it's happening, and I just, and I'm trying, but I just can't. And then, and then it's just another thing that I'm failing at, just another thing that I can't really get.</t>
         </is>
       </c>
     </row>
@@ -599,7 +842,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -622,178 +865,209 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Hello Mei Lin, it's good to see you again. I appreciate you coming back for a second session. Last time, we discussed some of the feelings of heaviness, fatigue, and loneliness you've been experiencing, as well as thoughts that have been troubling you. I want to start by checking in—how have you been feeling since our last conversation? Have there been any changes in your mood, energy levels, or sleep?</t>
+          <t>Hi Gabriella, it's good to see you again. I appreciate you coming back for another session. Last time, you shared quite a bit about how you've been feeling since your breakup and the difficulties you're experiencing with motivation and self-esteem. How have things been for you since we last talked?</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hi... Thanks for asking. Honestly, I think things haven't really gotten better. I still feel really tired all the time, and my sleep's still pretty bad. Sometimes I wake up in the middle of the night and can't fall back asleep. I guess the heaviness and feeling alone are still there, but maybe a little worse.</t>
+          <t>Hi, um, thanks. I guess... things are kind of the same, honestly. Like, I still feel pretty stuck most days. I’ve been trying to get out of the house more, like doing that waitressing thing last week, but it didn’t really make me feel better, you know? Just more nervous and kind of overwhelmed. I don’t know if I’m making any progress or just going in circles.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>I'm sorry to hear that things haven't improved and that you're feeling even more heaviness and loneliness. It sounds like these symptoms are persistent and quite challenging. Given what you've shared, I’d like to understand more about how you're coping with these feelings on a daily basis. For example, when you notice these feelings intensifying, what do you usually do? Do you find any ways to manage or distract yourself, or do you tend to internalize everything?</t>
+          <t>It sounds like you're putting in some effort by trying to get out and do new things, but you're feeling that it's not translating into feeling better, and maybe even making you feel more overwhelmed. When you think about the waitressing shift, what do you notice about your thoughts and feelings during or after that experience?</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Honestly, I just try to keep going, but I don’t do much to handle it. Sometimes I just sit alone and think about everything that’s wrong. I don't really talk to anyone about how I feel because I think they'll just worry or think I'm being dramatic. I try to focus on my classes, but it’s hard. Mostly, I just keep quiet and hope it will go away on its own, but it doesn’t.</t>
+          <t>Yeah, I guess that’s pretty accurate. Um, during the shift, I was really nervous—like, my stomach was doing flips, and I kept thinking I was messing up. I kept telling myself I wasn’t good enough or that I was slow, and I felt kinda embarrassed when I didn’t get things right. Afterward, I just felt... more down, like I failed again, even though everyone said it’s normal for a first shift. I keep thinking maybe I shouldn’t even bother trying if I’m just gonna mess up anyway. It’s like, I want to feel better, but I just end up feeling worse.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>It sounds like you're carrying a lot on your own and trying to manage these overwhelming feelings silently. Sitting alone and thinking about everything that feels wrong can sometimes make those feelings even heavier. You mentioned that focusing on your classes is difficult and that you hope things will improve on their own, but they haven't yet. 
-When you think about your future or your daily life, how do these persistent feelings and thoughts affect your motivation or your sense of hope? Do you find it harder to see things positively or to believe that things can get better?</t>
+          <t>It sounds like during that shift, your thoughts were quite negative—about your abilities and the way you’re perceived—and those thoughts led to feelings of embarrassment and disappointment afterward. You mentioned feeling like you’re just going in circles and that trying might be pointless because it leads to feeling worse. When you notice those thoughts, how much do you believe them on a scale from 0 to 100? For example, how strongly do you think "I'm just going to mess up" or "I'm not good enough"?</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Yeah, I guess I do feel less hopeful lately. Like, I used to be excited about my classes and my future, but now everything just feels so distant and impossible. Sometimes I think maybe I’m just not strong enough to handle all this. It’s like I’ve lost the motivation to try or believe that things will improve. It’s pretty discouraging, honestly.</t>
+          <t>Um, I’d say... probably around 75 or 80. Like, I know part of me knows I might just be being hard on myself, but another part feels really convinced that I’m just not cut out for these things, or that I’m just going to keep messing up no matter what. It’s kind of frustrating because I want to believe I can get better, but those thoughts feel so real sometimes. And honestly, it’s kind of exhausting to keep fighting that voice in my head.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Thank you for sharing that, Mei Lin. It’s understandable to feel that way when everything seems distant and impossible, especially when you're already dealing with so much. Losing motivation and hope can be really tough, and it’s a common experience in depression.
-Given how persistent these feelings are, I want to explore ways we might be able to help you regain some of that motivation and hope. But first, I’d like to understand more about what you’re hoping to achieve through our sessions. Are there specific changes or goals you’d like to work toward? For example, would you like to find ways to cope better, improve your sleep, or reconnect with activities or people you once enjoyed?</t>
+          <t>It’s understandable that those persistent, negative thoughts feel very convincing and exhausting. You’re caught between knowing they might not be entirely true and feeling overwhelmed by them anyway. When you think about trying to challenge these thoughts or tell yourself they might not be completely accurate, what kind of response do you usually have? Do you find it easy or hard to question or reframe those beliefs?</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Honestly, I just want to feel a little better. Like, I don’t expect to be totally fine, but maybe I could get some energy back or stop feeling so heavy all the time. I’d like to sleep better too, even if it’s just a little. I guess I also want to stop feeling so alone and be able to talk about what I’m going through without feeling like a burden. If I could do that, I think I’d feel more hopeful about everything.</t>
+          <t>Honestly, it’s pretty hard. I mean, I try to tell myself, like, “Maybe I just need more practice,” or “Everyone makes mistakes,” but then I think, yeah, but what if I really am just not good enough? Or what if I’m just fooling myself? It’s like, I want to believe I can change, but my mind keeps pulling me back to those doubts. It’s kind of like, I want to be more hopeful, but I just don’t feel it yet.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>That’s a very honest and thoughtful way to express your goals, Mei Lin. Wanting to feel a little better, regain some energy, improve your sleep, and connect more openly with others are all meaningful steps toward feeling more hopeful. It’s good to have clear, achievable aims like these, and they give us a foundation to work on together.
-As we move forward, we can explore some strategies to help you work toward these goals—things like small behavioral changes, coping skills, and perhaps ways to gradually build your support network. Does that sound like a helpful plan for now?</t>
+          <t>That’s a very honest and insightful reflection. It sounds like you’re aware of the possibility of change and even trying to hold onto hope, but those deep-seated doubts keep pulling you back into a negative mindset. When you’re caught in that cycle of doubt and hope, what do you usually do? Do you find yourself ruminating, withdrawing, or perhaps trying to distract yourself?</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Yes, that sounds helpful. I really want to try something different, even if it’s just small. I just don’t want to keep feeling like this forever.</t>
+          <t>Um, I think I mostly just ruminate, honestly. Like, I keep replaying everything in my head—what I said, what I did wrong, how I probably disappointed everyone, especially my mom. Sometimes I just want to distract myself, but I feel guilty about not doing anything productive or not trying hard enough to fix it. So, yeah, I guess I mostly just get stuck in my head, and that makes me feel even more tired and hopeless. It’s like I can’t really escape those thoughts, even if I want to.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>That’s a very positive mindset, Mei Lin. Even small steps can make a significant difference over time. I’m glad you’re open to trying new approaches, and I want you to know that progress often comes gradually. 
-Before we plan specific strategies, I’d like to check in on your current support system. Do you feel comfortable reaching out to someone—like a friend, family member, or counselor—if you need someone to talk to, especially on days when things feel overwhelming?</t>
+          <t>It sounds like your mind tends to get stuck in a loop of these negative thoughts, especially about disappointing your mom and feeling tired and hopeless. That rumination seems to drain your energy and make it harder to see a way forward. When you notice yourself ruminating, what do you think might help, even just a little, to break that cycle? Or what have you tried that maybe offers some relief, even temporarily?</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Honestly, I don’t really have anyone I feel comfortable talking to about this. My friends are busy, and I don’t want to bother my family with my problems. I guess I’ve just been trying to handle everything by myself. It’s kind of lonely, but I don’t see other options right now.</t>
+          <t>Honestly, I haven’t really figured out what works yet. Sometimes I try to distract myself by watching shows or scrolling on my phone, but then I just feel guilty because I’m not doing anything meaningful. Other times, I just sit there and think about everything, which makes it worse. I guess I haven’t found a good way to stop those thoughts from taking over. It’s like, I want to find something that can help me feel a little better, even if it’s just for a moment, but I don’t know what that is yet.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>It sounds like you’re feeling quite isolated, Mei Lin, and that reaching out feels difficult because you don’t want to burden others. That’s a common feeling when dealing with depression, and it’s understandable. Even if it’s hard to talk to people around you right now, I want to reassure you that support is available, and you don’t have to handle everything on your own.
-In our work together, we can explore ways for you to build a more supportive network gradually, and I can also suggest some coping strategies to help manage feelings of loneliness and heaviness. Would you be open to discussing some small steps you might take to connect with others or find additional support?</t>
+          <t>It makes sense that you're seeking something to help you feel even briefly better, but haven't quite found what works yet. That frustration is understandable. Sometimes, finding small, manageable activities that don’t feel overwhelming can be a helpful starting point. Have you noticed any activities or moments, even small ones, that have brought you a little relief or distraction in the past? Or perhaps things you’ve enjoyed before but haven't done recently?</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Maybe I could try talking to one of my friends, even if it’s just a little. I’ve never really opened up before, but I guess I could start. I don’t know if it will help, but I think I need to try something.</t>
+          <t>Hmm, I guess... I used to like drawing or writing in my journal, but I haven't really done either in a while. When I was younger, I’d spend hours just sketching or writing stories, and it made me forget about everything for a bit. But now, I just feel like I don’t have the energy or motivation to do those things anymore. It’s like, even if I want to, I just can’t seem to get started or find the interest. I wonder if I should try again, but I’m not sure if it’ll make a difference.</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>That’s a very brave and thoughtful decision, Mei Lin. Starting to open up, even just a little, can be a meaningful step toward feeling less alone and gaining support. It’s understandable to feel uncertain about how it will help, but taking that first step can sometimes lead to relief and connection that you might not expect.
-As you consider reaching out, perhaps you could think about sharing just a small part of how you’ve been feeling, or even asking your friend for some support or understanding. Would you like some guidance on how to approach that conversation or ideas for what to say?</t>
+          <t>Reconnecting with activities like drawing or journaling that once brought you some peace sounds like a meaningful idea. It’s understandable to feel hesitant, especially when motivation and energy are low. Sometimes, just allowing yourself to engage in these activities without pressure—maybe for a few minutes—can help gently break the cycle of rumination. How do you feel about giving yourself permission to try again, even if it’s just a small step?</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Yeah, I think I might need some help with what to say. I’ve never really done this before, so I’m not sure how to start or what to say exactly.</t>
+          <t>I guess I could try, yeah. Like, maybe I don’t have to do it perfectly or spend hours on it. Just, you know, a little bit, just to see if it helps me feel a bit more... grounded or something. It’s just hard to believe it’ll actually make a difference, but I suppose I can give it a shot. I don’t want to keep feeling like this all the time, so maybe it’s worth trying.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>That's completely understandable, Mei Lin. Opening up for the first time can feel intimidating, but it’s a positive step, and I can help you prepare. Sometimes, starting with simple, honest words can make it easier. For example, you might say something like, “I’ve been feeling really overwhelmed and tired lately, and I’ve been struggling with some heavy feelings. I don’t expect you to have all the answers, but I just need someone to listen.” 
-Would you like to practice a few sentences or explore different ways you might begin that conversation?</t>
+          <t>That sounds like a very reasonable and compassionate approach—giving yourself permission to engage in those activities without the pressure of doing it perfectly. Even small steps can sometimes lead to noticeable changes over time. If you decide to try drawing or journaling, perhaps setting a timer for just a few minutes could make it feel more manageable. Would you be willing to share how it goes next time, or if you notice any small shifts in how you’re feeling?</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Yeah, I think practicing might help. I want to say something, but I’m worried I’ll sound weird or like I’m just complaining.</t>
+          <t>Yeah, I think I could do that. I mean, it’s not like I have much else going on right now, so I might as well try. I guess I’ll start with just a few minutes, like you said, and see if it helps. It’s kind of embarrassing to even admit I’m trying this, but maybe it’s worth a shot. Thanks for suggesting it. I’ll let you know how it goes next time.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>That’s a very common concern, Mei Lin, and it’s understandable to worry about how you’ll come across. Remember, your feelings are valid, and sharing them is a sign of strength, not weakness. 
-Let’s try to craft a simple, genuine way to start that feels comfortable for you. Would you like to try saying, “Hey, I’ve been feeling a bit overwhelmed lately, and I just need someone to listen,” or would you prefer to start even more casually?</t>
+          <t>That’s a very brave and honest decision, Gabriella. Remember, taking even small steps like that is a positive move forward, and there’s no shame in trying. It’s all about finding what works for you, one step at a time. I look forward to hearing how it goes next time. For now, is there anything else you’d like to share or explore today?</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Maybe I could say, "Hey, I’ve been feeling really tired and kind of down lately, and I just want to talk to someone, if that’s okay." Is that okay?</t>
+          <t>Honestly, I’m not sure. I feel like I’ve been just going over the same stuff in my head, and I don’t know if there’s anything new I want to talk about. But maybe, I guess, I’m still struggling with feeling like I’m not good enough—like, even if I try those little things, I still doubt myself a lot. It’s kind of frustrating because I want to believe I can get better, but I just don’t know how to really believe it yet. Maybe that’s something I need to work on more.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>That’s a very thoughtful and gentle way to start, Mei Lin. It honestly communicates your feelings without sounding demanding or dramatic, and it shows your willingness to connect. Saying, "Hey, I’ve been feeling really tired and kind of down lately, and I just want to talk to someone, if that’s okay," is a good way to open the door for support.
-Would you like to practice how you might continue the conversation if your friend responds positively? Or if you prefer, we can talk about what you might say if they seem unsure or don’t respond right away.</t>
+          <t>It’s understandable to feel that way, Gabriella. Doubting yourself and feeling not good enough can be very persistent, especially when those thoughts have been part of your experience for a while. Recognizing that this is something you want to work on is an important insight. Building that belief in yourself often takes time and small successes, even if they feel minor at first. 
+Would you be open to exploring some strategies or exercises that might help gradually strengthen your self-belief? Or perhaps discussing ways to challenge those doubts when they come up?</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>I think I’d like to practice what I might say next, just in case they ask me more or want to know how I’m feeling. I want to be honest, but I don’t want to scare them off.</t>
+          <t>Yeah, I think I’d be willing to try that. I mean, I don’t really know how to challenge those doubts, though. It’s like, I hear them, and I just believe them most of the time. But maybe if I had some kind of way to, I don’t know, talk back to them or remind myself of other things, it could help. I just don’t really know where to start with that, or if it even works.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>That’s a very thoughtful approach, Mei Lin. Honesty is important, and it’s also good to be mindful of how much you share, especially when opening up for the first time. 
-If your friend asks, “How are you feeling?” or “What’s going on?” you might say something like, “Honestly, I’ve been feeling pretty overwhelmed and tired, and I’ve been having a hard time sleeping and concentrating. It’s been tough to shake the heaviness, and sometimes I feel pretty lonely. I don’t want to burden anyone, but I think I need to talk about it to start feeling a bit better.” 
-Would you like to practice saying that, or do you want to try a slightly different way to express it?</t>
+          <t>That’s a very honest and thoughtful reflection. Challenging those doubts can feel difficult, especially when they seem so convincing. A common approach in CBT is to identify these negative thoughts, examine the evidence for and against them, and then develop more balanced or realistic perspectives. It’s like having a conversation with that inner critic, where you gently question its assumptions and remind yourself of your strengths or positive qualities.
+Would you like to work through an example of one of your doubts—say, the thought “I’m not good enough”—and see how we might challenge it together?</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>I think I can try saying that. It sounds honest but not too heavy. Thanks for helping me practice.</t>
+          <t>Yeah, I think that could be helpful. I mean, I guess I do have some moments where I realize I’m not as terrible as I think—I mean, I did get through the shift, even if I was nervous and slow. But then I just tell myself that it was just luck or that I was lucky they were patient with me. So, I don’t know, how do I really challenge that kind of thought? It feels like I’m just making excuses, but I don’t want to believe I’m just fooling myself either.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>You're very welcome, Mei Lin. I'm glad you feel comfortable trying that out. Remember, sharing even a little of how you're feeling can be a powerful step toward feeling less alone and gaining support. Whenever you're ready, I hope you'll give it a try. 
-In the meantime, if you want to talk more about how to handle different reactions or need more support in preparing, I’m here for you. Would you like to discuss any other concerns or questions right now?</t>
+          <t>That’s a very insightful observation—you recognize your efforts and some moments of competence, but then dismiss them as luck or patience. Challenging that kind of thought involves looking at the evidence more objectively and considering alternative explanations. 
+For example, when you think, “It was just luck,” you can ask yourself, “What evidence do I have that supports or contradicts that?” Have there been times when you managed tasks or handled situations well, even if you were nervous? Or perhaps moments where others acknowledged your effort or progress? 
+Would you like to try framing some evidence for and against that thought?</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>No, I think I want to wait and think about it a bit more. Thanks for your help and understanding.</t>
+          <t>Yeah, I suppose there have been times when I did okay, even if I was nervous. Like, I did remember some of the orders, and people didn’t seem too annoyed with me. And my mom said I was doing fine, even if I felt like I was messing up. But then I think, maybe she’s just being nice or trying to make me feel better. So, I guess I can see that there’s some truth in what you’re saying, but it’s hard to really believe it.</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>That sounds like a good plan, Mei Lin. Take your time to think it over, and remember, you’re doing a very brave thing by considering reaching out. I’m here whenever you feel ready, and I look forward to our next conversation. Take care, and see you next time.</t>
+          <t>Exactly, Gabriella. You’re already doing a great job of examining the evidence—recognizing that you did some things right, and that others, like your mom, offered reassurance. The challenge is in balancing that evidence against the doubts that tell you otherwise. It’s normal for those doubts to feel very strong, especially when you’re feeling low. 
+A helpful next step can be to create a more balanced thought—something like, “I may have been nervous and made some mistakes, but I also remembered some things and handled some situations okay.” Does that resonate with you? Would you like to try crafting a balanced thought together?</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
+        <is>
+          <t>Yes, I think I could try that. It’s kind of strange, because part of me still feels like I’m just pretending or that I’m fooling myself, but I guess I can see that I did some things right. Maybe I can tell myself that even if I was nervous, I still managed to do some things okay, and that’s not nothing. I’ll try to keep that in mind next time those doubts come up. Thanks for helping me see that there’s a different way to look at it.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>That’s a really thoughtful and balanced way to approach those doubts, Gabriella. Acknowledging both the difficulties and the successes can help you build a more realistic and compassionate view of yourself. Remember, challenging negative thoughts is a process, and it’s normal for doubts to linger. With practice, it can become easier to see your efforts and progress more clearly. 
+Would you like to set a small goal for yourself before our next session, maybe related to practicing this kind of balanced thinking or engaging in one of your favorite activities again?</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Yeah, I think I’d like to try that. Maybe I can practice challenging my doubts when they come up, just like we talked about, and also try to do a little drawing or writing in my journal. Even if it’s just for a few minutes, I think it might help me feel a bit more connected to myself. I’ll see how it goes, and I’ll let you know next time. Thanks for all the support today.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>That sounds like a very practical and compassionate plan, Gabriella. Practicing challenging your doubts when they arise and reconnecting with your creative outlets are excellent steps toward feeling more grounded and confident. Remember, progress can be gradual, and every small effort counts. I look forward to hearing how it goes next time. 
+Thank you for sharing honestly today. See you next time.</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Thank you. I appreciate it. I’ll try my best. See you next time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>You're very welcome, Gabriella. I admire your willingness to try and your thoughtful approach. Take care, and I look forward to hearing about your progress next time. See you then.</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>Goodbye.</t>
         </is>
@@ -810,7 +1084,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -833,192 +1107,209 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Hello Mei Lin, it's good to see you again. I appreciate you coming back for our third session. Last time, we discussed how you've been feeling with persistent fatigue, sleep difficulties, feelings of heaviness, loneliness, and some thoughts about giving up. You mentioned that these feelings haven't improved much and that you're still struggling with motivation and hope.
-How have you been feeling since our last conversation? Have there been any changes in your mood, energy, or sleep patterns?</t>
+          <t>Hi Gabriella, it’s good to see you again. I appreciate you coming back for another session. Last time, you shared quite a bit about how you’ve been feeling since your breakup and the difficulties you’re experiencing with motivation and self-esteem. How have things been for you since we last talked?</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hi... Thanks for asking. Honestly, I think things are still pretty much the same. I haven't really felt any better, and my energy is still really low. Sleep is still a problem—I wake up a lot during the night or sleep too much but still feel tired. The heaviness and feeling alone are still there, maybe even a bit worse.</t>
+          <t>Hi, thanks. Um, honestly, not much has changed. I still feel pretty stuck most days, you know? I tried going back to that waitressing thing last week, but honestly, it just made me more nervous and overwhelmed. I don’t know if I’m really making any progress or just going in circles, really. It’s kind of frustrating.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>I'm sorry to hear that you're still feeling this way, Mei Lin. It sounds like these symptoms are quite persistent and distressing. Given what you've shared, it might help to explore how you're coping with these feelings on a daily basis. When you notice these feelings intensifying, what do you usually do? Do you find any ways to manage or distract yourself, or do you tend to internalize everything?</t>
+          <t>It sounds like despite your efforts to get out there and try new things, you're feeling like it's not helping much and perhaps even making you feel more overwhelmed. When you think about that waitressing shift, what thoughts or feelings come up during or after the experience?</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Honestly, I mostly just try to push through it. I don't really do much to manage it. Sometimes I sit alone and think about everything that's wrong. I don't really talk to anyone about how I feel because I think they'll just worry or think I'm being dramatic. I just keep quiet and hope it will go away, but it doesn't.</t>
+          <t>Yeah, exactly. During the shift, I was, um, really nervous—like, my stomach was doing flips, and I kept thinking I was messing up. I kept telling myself I wasn’t good enough or that I was slow, and I felt kind of embarrassed when I didn’t get things right. Afterward, I just felt… more down, like I failed again, even though everyone said it’s normal for a first shift. I keep thinking maybe I shouldn’t even bother trying if I’m just gonna mess up anyway. It’s like, I want to feel better, but I just end up feeling worse.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>It sounds like you're carrying a lot on your own, Mei Lin, and trying to handle these overwhelming feelings silently. Sitting alone and dwelling on everything that feels wrong can sometimes make those feelings even heavier. You mentioned that focusing on your classes is difficult and that you hope things will improve on their own, but they haven't yet. 
-When you think about your future or your daily life, how do these persistent feelings and thoughts affect your motivation or your sense of hope? Do you find it harder to see things positively or to believe that things can get better?</t>
+          <t>It sounds like during the shift, your thoughts were quite negative—about your abilities and the way you're perceived—and those thoughts led to feelings of embarrassment and disappointment afterward. You mentioned feeling like you're just going in circles and that trying might be pointless because it leads to feeling worse. When you notice those thoughts, how much do you believe them on a scale from 0 to 100? For example, how strongly do you think "I'm just going to mess up" or "I'm not good enough"?</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Yeah, I guess I do feel less hopeful lately. Like, I used to be excited about my classes and future, but now everything feels so distant and impossible. Sometimes I think maybe I’m just not strong enough to handle all this. It’s like I’ve lost the motivation to try or believe that things will improve. It’s pretty discouraging, honestly.</t>
+          <t>Um, I’d say… probably around 75 or 80. Like, I know part of me knows I might just be being hard on myself, but another part feels really convinced that I’m just not cut out for these things, or that I’m just going to keep messing up no matter what. It’s kind of frustrating because I want to believe I can get better, but those thoughts feel so real sometimes. And honestly, it’s kind of exhausting to keep fighting that voice in my head.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Thank you for sharing that, Mei Lin. It’s completely understandable to feel less hopeful when everything seems distant and impossible, especially under the weight of what you're experiencing. Feeling a loss of motivation and hope can be very tough, and it’s a common part of depression. 
-Given how persistent these feelings are, I want to explore ways we might be able to help you regain some of that motivation and hope. Would you be open to discussing some strategies to help you cope better, or perhaps looking at some small steps you might take to start feeling a bit more hopeful?</t>
+          <t>That’s very understandable. Those persistent, negative thoughts can feel very convincing and exhausting. You’re caught between knowing they might not be entirely true and feeling overwhelmed by them anyway. When you think about trying to challenge these thoughts or tell yourself they might not be completely accurate, what kind of response do you usually have? Do you find it easy or hard to question or reframe those beliefs?</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Yeah, I think I’d like that. I really just want to feel a little better, even if it’s just a little.</t>
+          <t>Honestly, it’s pretty hard. I mean, I try to tell myself, like, “Maybe I just need more practice,” or “Everyone makes mistakes,” but then I think, yeah, but what if I really am just not good enough? Or what if I’m just fooling myself? It’s like, I want to believe I can change, but my mind keeps pulling me back to those doubts. It’s kind of like, I want to be more hopeful, but I just don’t feel it yet.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>That’s a very positive and realistic goal, Mei Lin. Wanting to feel a bit better and taking small steps toward that is a great approach. Sometimes, even minor improvements can make a big difference over time. 
-Before we discuss specific strategies, I’d like to understand more about what you’re hoping to achieve through our sessions. For example, are there particular areas—like sleep, motivation, or feeling less lonely—that you’d like us to focus on? Or any specific changes you’d like to see in how you’re feeling or handling things?</t>
+          <t>That’s a very honest and insightful reflection. It sounds like you’re aware of the possibility of change and even trying to hold onto hope, but those deep-seated doubts keep pulling you back into a negative mindset. When you’re caught in that cycle of doubt and hope, what do you usually do? Do you find yourself ruminating, withdrawing, or perhaps trying to distract yourself?</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>I guess I just want to feel more like myself again. Like, I want to have some energy and not feel so heavy all the time. Sleep would be good too, even if it’s just a little better. And I really want to stop feeling so alone and be able to talk about what I’m going through without feeling like a burden. If I could do that, I think I’d feel more hopeful about everything.</t>
+          <t>Yeah, I think I mostly just ruminate, honestly. Like, I keep replaying everything in my head—what I said, what I did wrong, how I probably disappointed everyone, especially my mom. Sometimes I just want to distract myself, but I feel guilty about not doing anything productive or not trying hard enough to fix it. So, yeah, I guess I mostly just get stuck in my head, and that makes me feel even more tired and hopeless. It’s like, I can’t really escape those thoughts, even if I want to.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Those are really meaningful goals, Mei Lin—wanting to regain your energy, improve your sleep, and feel less alone by being able to share your feelings. It’s a good foundation for us to work from. 
-In our next steps, we can explore some practical strategies to help you work toward these goals. Things like small behavioral changes, coping skills, and ways to gradually build your support network could be helpful. Does that sound like a good plan for now?</t>
+          <t>It sounds like your mind tends to get stuck in a loop of these negative thoughts, especially about disappointing your mom and feeling tired and hopeless. That rumination seems to drain your energy and make it harder to see a way forward. When you notice yourself ruminating, what do you think might help, even just a little, to break that cycle? Or what have you tried that maybe offers some relief, even temporarily?</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Yes, that sounds good. I really want to try something different, even if it’s just small. I just don’t want to keep feeling like this forever.</t>
+          <t>Honestly, I haven’t really figured out what works yet. Sometimes I try to distract myself by watching shows or scrolling on my phone, but then I just feel guilty because I’m not doing anything meaningful. Other times, I just sit there and think about everything, which makes it worse. I guess I haven’t found a good way to stop those thoughts from taking over. It’s like, I want to find something that can help me feel a little better, even if it’s just for a moment, but I don’t know what that is yet.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>That’s a very hopeful outlook, Mei Lin. Even small changes can lead to meaningful improvements over time. I’m glad you’re open to trying different approaches, and I want you to remember that progress often happens gradually. 
-Before we get into specific strategies, I’d like to check in about your current support system. Do you feel comfortable reaching out to someone—like a friend, family member, or counselor—if you need support or someone to talk to, especially on days when things feel overwhelming?</t>
+          <t>It makes sense that you're seeking something to help you feel even briefly better, but haven't quite found what works yet. That frustration is understandable. Sometimes, finding small, manageable activities that don’t feel overwhelming can be a helpful starting point. Have you noticed any activities or moments, even small ones, that have brought you a little relief or distraction in the past? Or perhaps things you’ve enjoyed before but haven't done recently?</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Honestly, I don’t really have anyone I feel comfortable talking to about this. My friends are busy, and I don’t want to bother my family with my problems. I’ve been trying to handle everything myself. It’s pretty lonely, but I don’t see many other options right now.</t>
+          <t>Hmm, I guess... I used to like drawing or writing in my journal, but I haven't really done either in a while. When I was younger, I’d spend hours just sketching or writing stories, and it made me forget about everything for a bit. But now, I just feel like I don’t have the energy or motivation to do those things anymore. It’s like, even if I want to, I just can’t seem to get started or find the interest. I wonder if I should try again, but I’m not sure if it’ll make a difference.</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>It sounds like you're feeling quite isolated, Mei Lin, and that reaching out feels difficult because you don’t want to burden others. That’s a common feeling when dealing with depression, and it’s understandable. Even if it’s hard to talk to people around you right now, I want to reassure you that support is available, and you don’t have to handle everything all on your own.
-In our work together, we can explore ways for you to gradually build a more supportive network. Also, I can suggest some coping strategies to help manage feelings of loneliness and heaviness. Would you be open to discussing some small steps you might take to connect with others or find additional support?</t>
+          <t>Reconnecting with activities like drawing or journaling that once brought you some peace sounds like a meaningful idea. It’s understandable to feel hesitant, especially when motivation and energy are low. Sometimes, just allowing yourself to engage in these activities without pressure—maybe for a few minutes—can help gently break the cycle of rumination. How do you feel about giving yourself permission to try again, even if it’s just a small step?</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Maybe I could try talking to one of my friends, even if it’s just a little. I’ve never really opened up before, but I guess I could start. I don’t know if it will help, but I think I need to try something.</t>
+          <t>I guess I could try, yeah. Like, maybe I don’t have to do it perfectly or spend hours on it. Just, you know, a little bit, just to see if it helps me feel a bit more... grounded or something. It’s just hard to believe it’ll actually make a difference, but I suppose I can give it a shot. I don’t want to keep feeling like this all the time, so maybe it’s worth trying.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>That’s a very brave and thoughtful decision, Mei Lin. Starting to open up, even just a little, can be a meaningful step toward feeling less alone and gaining support. It’s understandable to feel uncertain about how it will help, but taking that first step can sometimes lead to relief and connection that you might not expect.
-As you consider reaching out, perhaps you could think about sharing just a small part of how you’ve been feeling, or even asking your friend for some support or understanding. Would you like some guidance on how to approach that conversation or ideas for what to say?</t>
+          <t>That sounds like a very reasonable and compassionate approach—giving yourself permission to engage in those activities without the pressure of doing it perfectly. Even small steps can sometimes lead to noticeable changes over time. If you decide to try drawing or journaling, perhaps setting a timer for just a few minutes could make it feel more manageable. Would you be willing to share how it goes next time, or if you notice any small shifts in how you’re feeling?</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Yeah, I think I might need some help with what to say. I’ve never really done this before, so I’m not sure how to start or what to say exactly.</t>
+          <t>Yeah, I think I could do that. I mean, it’s not like I have much else going on right now, so I might as well try. I guess I’ll start with just a few minutes, like you said, and see if it helps. It’s kind of embarrassing to even admit I’m trying this, but maybe it’s worth a shot. Thanks for suggesting it. I’ll let you know how it goes next time.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>That’s very understandable, Mei Lin. Opening up for the first time can feel intimidating, but it’s a brave step, and I can help you prepare. Sometimes, starting with simple, honest words makes it easier. For example, you might say, “I’ve been feeling really overwhelmed and tired lately, and I’ve been struggling with some heavy feelings. I don’t expect you to have all the answers, but I just need someone to listen.” 
-Would you like to practice a few sentences or explore different ways you might begin that conversation?</t>
+          <t>That’s a very brave and honest decision, Gabriella. Remember, taking even small steps like that is a positive move forward, and there’s no shame in trying. It’s all about finding what works for you, one step at a time. I look forward to hearing how it goes next time. For now, is there anything else you’d like to share or explore today?</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Yes, I think practicing might help. I want to say something, but I’m worried I’ll sound weird or like I’m just complaining.</t>
+          <t>I guess, um, I don’t know. I feel like I’ve just been going over the same stuff in my head, and I’m not really sure if there’s anything new I want to talk about. But I guess I’m still struggling with feeling like I’m not good enough—like, even if I do those little things, I still doubt myself a lot. It’s kind of frustrating because I want to believe I can get better, but I just don’t know how to really believe it yet. Maybe that’s something I need to work on more.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>That’s a very common concern, Mei Lin, and it’s understandable to worry about how you’ll come across. Remember, your feelings are valid, and sharing them is a sign of strength, not weakness. 
-Let’s try to craft a simple, genuine way to start that feels comfortable for you. Would you like to try saying, “Hey, I’ve been feeling a bit overwhelmed lately, and I just need someone to listen,” or would you prefer to start even more casually?</t>
+          <t>It’s completely understandable to feel that way, Gabriella. Doubting yourself and feeling not good enough can be very persistent, especially when those thoughts have been part of your experience for a while. Recognizing that this is something you want to work on is an important insight. Building that belief in yourself often takes time and small successes, even if they feel minor at first.
+Would you be open to exploring some strategies or exercises that might help gradually strengthen your self-belief? Or perhaps discussing ways to challenge those doubts when they come up?</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Maybe I could say, "Hey, I’ve been feeling really tired and kind of down lately, and I just want to talk to someone, if that’s okay." Is that okay?</t>
+          <t>Yeah, I think I’d be willing to try that. I mean, I don’t really know how to challenge those doubts, though. It’s like, I hear them, and I just believe them most of the time. But maybe if I had some kind of way to, I don’t know, talk back to them or remind myself of other things, it could help. I just don’t really know where to start with that, or if it even works.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>That’s a very thoughtful and gentle way to start, Mei Lin. It honestly communicates your feelings without sounding demanding or dramatic, and it shows your willingness to connect. Saying, "Hey, I’ve been feeling really tired and kind of down lately, and I just want to talk to someone, if that’s okay," is a good way to open the door for support.
-Would you like to practice how you might continue the conversation if your friend responds positively? Or if you prefer, we can talk about what you might say if they seem unsure or don’t respond right away.</t>
+          <t>That’s a very honest and thoughtful reflection. Challenging those doubts can feel difficult, especially when they seem so convincing. A common approach in CBT is to identify these negative thoughts, examine the evidence for and against them, and then develop more balanced or realistic perspectives. It’s like having a conversation with that inner critic, where you gently question its assumptions and remind yourself of your strengths or positive qualities.
+Would you like to work through an example of one of your doubts—say, the thought “I’m not good enough”—and see how we might challenge it together?</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>I think I’d like to practice what I might say next, just in case they ask me more or want to know how I’m feeling. I want to be honest, but I don’t want to scare them off.</t>
+          <t>Yeah, I think that could be helpful. I mean, I guess I do have some moments where I realize I’m not as terrible as I think—I mean, I did get through the shift, even if I was nervous and slow. But then I just tell myself that it was just luck or that I was lucky they were patient with me. So, I don’t know, how do I really challenge that kind of thought? It feels like, I’m just making excuses, but I don’t want to believe I’m just fooling myself either.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>That’s a very thoughtful approach, Mei Lin. Honesty is important, and it’s also good to be mindful of how much you share, especially when opening up for the first time. 
-If your friend asks, “How are you feeling?” or “What’s going on?” you might say something like, “Honestly, I’ve been feeling pretty overwhelmed and tired, and I’ve been having a hard time sleeping and concentrating. It’s been tough to shake the heaviness, and sometimes I feel pretty lonely. I don’t want to burden anyone, but I think I need to talk about it to start feeling a bit better.” 
-Would you like to practice saying that, or do you want to try a slightly different way to express it?</t>
+          <t>That’s a very insightful observation—you recognize your efforts and some moments of competence, but then dismiss them as luck or patience. Challenging that kind of thought involves looking at the evidence more objectively and considering alternative explanations. 
+For example, when you think, “It was just luck,” you can ask yourself, “What evidence do I have that supports or contradicts that?” Have there been times when you managed tasks or handled situations well, even if you were nervous? Or perhaps moments where others acknowledged your effort or progress? 
+Would you like to try framing some evidence for and against that thought?</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>I think I can try saying that. It sounds honest but not too heavy. Thanks for helping me practice.</t>
+          <t>Yeah, I suppose there have been times when I did okay, even if I was nervous. Like, I did remember some of the orders, and people didn’t seem too annoyed with me. And my mom said I was doing fine, even if I felt like I was messing up. But then I think, maybe she’s just being nice or trying to make me feel better. So, I guess I can see that there’s some truth in what you’re saying, but it’s hard to really believe it.</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>You're very welcome, Mei Lin. I'm glad you feel comfortable trying that out. Remember, sharing even a little of how you're feeling can be a powerful step toward feeling less alone and gaining support. Whenever you're ready, I hope you'll give it a try. 
-In the meantime, if you want to talk more about how to handle different reactions or need more support in preparing, I’m here for you. Would you like to discuss any other concerns or questions right now?</t>
+          <t>Exactly, Gabriella. You’re already doing a great job of examining the evidence—recognizing that you did some things right, and that others, like your mom, offered reassurance. The challenge is in balancing that evidence against the doubts that tell you otherwise. It’s normal for those doubts to feel very strong, especially when you’re feeling low.
+A helpful next step can be to create a more balanced thought—something like, “I may have been nervous and made some mistakes, but I also remembered some things and handled some situations okay.” Does that resonate with you? Would you like to try crafting a balanced thought together?</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>No, I think I want to wait and think about it a bit more. Thanks for your help and understanding.</t>
+          <t>Yes, I think I could try that. It’s kind of strange, because part of me still feels like I’m just pretending or that I’m fooling myself, but I guess I can see that I did some things right. Maybe I can tell myself that even if I was nervous, I still managed to do some things okay, and that’s not nothing. I’ll try to keep that in mind next time those doubts come up. Thanks for helping me see that there’s a different way to look at it.</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>That sounds like a good plan, Mei Lin. Take your time to think it over, and remember, you’re doing a very brave thing by considering reaching out. I’m here whenever you feel ready, and I look forward to our next conversation. Take care, and see you next time.</t>
+          <t>That’s a very thoughtful and balanced way to approach those doubts, Gabriella. Acknowledging both the difficulties and the successes can help you build a more realistic and compassionate view of yourself. Remember, challenging negative thoughts is a process, and it’s normal for doubts to linger. With practice, it can become easier to see your efforts and progress more clearly.
+Would you like to set a small goal for yourself before our next session, maybe related to practicing this kind of balanced thinking or engaging in one of your favorite activities again?</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
+        <is>
+          <t>Yeah, I think I’d like to try that. Maybe I can practice challenging my doubts when they come up, just like we talked about, and also try to do a little drawing or writing in my journal. Even if it’s just for a few minutes, I think it might help me feel a bit more connected to myself. I’ll see how it goes, and I’ll let you know next time. Thanks for all the support today.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>That sounds like a very practical and compassionate plan, Gabriella. Practicing challenging your doubts when they arise and reconnecting with your creative outlets are excellent steps toward feeling more grounded and confident. Remember, progress can be gradual, and every small effort counts. I look forward to hearing how it goes next time.
+Thank you for sharing honestly today. See you next time.</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Thank you. I appreciate it. I’ll try my best. See you next time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>You're very welcome, Gabriella. I admire your willingness to try and your thoughtful approach. Take care, and I look forward to hearing about your progress next time. See you then.</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>Goodbye.</t>
         </is>
@@ -1027,22 +1318,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>